<commit_message>
change names and units, by Anita
</commit_message>
<xml_diff>
--- a/data/fq_variables.xlsx
+++ b/data/fq_variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajpelu/Library/CloudStorage/GoogleDrive-ajperez@go.ugr.es/My Drive/MS/DP/2024_DP_AVLASA/dp_avlasa_sylvestris/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABE609E-ED77-2742-9C87-61A3676D99FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5025E707-4EA2-1D46-83C0-3F9723938D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18400" yWindow="500" windowWidth="51200" windowHeight="27020" xr2:uid="{F3C35693-398C-2E4E-BB77-18D988B4F79B}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="27020" xr2:uid="{F3C35693-398C-2E4E-BB77-18D988B4F79B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
   <si>
     <t>p_h_k_cl</t>
   </si>
@@ -100,15 +100,6 @@
     <t>mg/L</t>
   </si>
   <si>
-    <t>Sulphate</t>
-  </si>
-  <si>
-    <t>Bicarbonate</t>
-  </si>
-  <si>
-    <t>Total N</t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
@@ -139,12 +130,6 @@
     <t>Field capacity</t>
   </si>
   <si>
-    <t>pH KCl</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>id_var</t>
   </si>
   <si>
@@ -188,6 +173,48 @@
   </si>
   <si>
     <t>S14</t>
+  </si>
+  <si>
+    <t>measurementMethod</t>
+  </si>
+  <si>
+    <t>pH measured in KCl</t>
+  </si>
+  <si>
+    <t>Electrochemical method</t>
+  </si>
+  <si>
+    <t>Sulphate content</t>
+  </si>
+  <si>
+    <t>Ion chromatography</t>
+  </si>
+  <si>
+    <t>Bicarbonate content</t>
+  </si>
+  <si>
+    <t>Volumetric method</t>
+  </si>
+  <si>
+    <t>Content of total N</t>
+  </si>
+  <si>
+    <t>Dumas method</t>
+  </si>
+  <si>
+    <t>ICP-MS</t>
+  </si>
+  <si>
+    <t>Spectrophotometry</t>
+  </si>
+  <si>
+    <t>Calculation</t>
+  </si>
+  <si>
+    <t>Densimetry</t>
+  </si>
+  <si>
+    <t>Gravimetry</t>
   </si>
 </sst>
 </file>
@@ -546,21 +573,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B294078E-35FA-8D45-A01E-61D0A9471583}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="296" zoomScaleNormal="296" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="176" zoomScaleNormal="176" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
@@ -571,21 +599,27 @@
       <c r="D1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -593,10 +627,13 @@
       <c r="C3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -607,156 +644,192 @@
       <c r="D4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>